<commit_message>
Final version - UPDATE
Final version with test screenshot
New code updated & compiled
</commit_message>
<xml_diff>
--- a/Testbench/testing_project_rl.xlsx
+++ b/Testbench/testing_project_rl.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\PFRL_pizzamiglio_prisciantelli\Testbench\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\BAKUP_RL_SERIO\PFRL_pizzamiglio_prisciantelli\Testbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1E1370-5009-4C2E-9F6E-BDC3070C3FEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D129F15-549E-4813-AD4C-31A3CAA3ED78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{1F41BA3C-3259-4399-9982-2D19E066B754}"/>
+    <workbookView xWindow="5760" yWindow="2232" windowWidth="17280" windowHeight="10074" xr2:uid="{1F41BA3C-3259-4399-9982-2D19E066B754}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="60">
   <si>
     <t>Testing - Project Reti Logiche</t>
   </si>
@@ -220,7 +220,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,8 +260,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +300,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -305,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -317,13 +331,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -640,24 +656,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53D9802-2C2B-4024-8462-0F2750AE00AA}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="60.9453125" customWidth="1"/>
-    <col min="3" max="5" width="25.26171875" customWidth="1"/>
+    <col min="3" max="5" width="25.26171875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14.9453125" customWidth="1"/>
     <col min="7" max="8" width="22.578125" customWidth="1"/>
     <col min="9" max="9" width="35.20703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
@@ -712,15 +728,14 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5">
@@ -729,18 +744,17 @@
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5">
@@ -749,18 +763,17 @@
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5">
@@ -775,12 +788,11 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5">
@@ -795,12 +807,11 @@
       <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5">
@@ -815,29 +826,27 @@
       <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5">
@@ -852,12 +861,11 @@
       <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5">
@@ -872,12 +880,11 @@
       <c r="D14" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5">
@@ -892,12 +899,11 @@
       <c r="D15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5">
@@ -912,14 +918,13 @@
       <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16" s="7"/>
+      <c r="F16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5">
         <v>12</v>
       </c>
@@ -932,14 +937,13 @@
       <c r="D17" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17" s="7"/>
+      <c r="F17" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5">
         <v>13</v>
       </c>
@@ -952,13 +956,17 @@
       <c r="D18" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" s="6"/>
+      <c r="F18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C19" t="s">
@@ -967,9 +975,11 @@
       <c r="D19" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F19" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5">
         <v>15</v>
       </c>
@@ -982,9 +992,11 @@
       <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F20" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5">
         <v>16</v>
       </c>
@@ -997,9 +1009,11 @@
       <c r="D21" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F21" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5">
         <v>17</v>
       </c>
@@ -1012,9 +1026,11 @@
       <c r="D22" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5">
         <v>18</v>
       </c>
@@ -1027,9 +1043,11 @@
       <c r="D23" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F23" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5">
         <v>19</v>
       </c>
@@ -1042,9 +1060,9 @@
       <c r="D24" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5">
         <v>20</v>
       </c>
@@ -1057,13 +1075,13 @@
       <c r="D25" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5">
         <v>21</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C26" t="s">
@@ -1072,13 +1090,13 @@
       <c r="D26" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5">
         <v>22</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C27" t="s">
@@ -1087,13 +1105,13 @@
       <c r="D27" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="5">
         <v>23</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C28" t="s">
@@ -1104,7 +1122,7 @@
       </c>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="5">
         <v>24</v>
       </c>
@@ -1119,11 +1137,11 @@
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="5">
         <v>25</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C30" t="s">
@@ -1134,11 +1152,11 @@
       </c>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="5">
         <v>26</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C31" t="s">
@@ -1149,11 +1167,11 @@
       </c>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="5">
         <v>27</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>51</v>
       </c>
       <c r="F32" s="6"/>
@@ -1171,7 +1189,9 @@
       <c r="D33" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="8"/>
+      <c r="F33" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="5">
@@ -1180,7 +1200,9 @@
       <c r="B34" t="s">
         <v>47</v>
       </c>
-      <c r="F34" s="8"/>
+      <c r="F34" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="5">
@@ -1190,7 +1212,9 @@
         <v>48</v>
       </c>
       <c r="C35" s="3"/>
-      <c r="F35" s="8"/>
+      <c r="F35" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="5">
@@ -1199,7 +1223,9 @@
       <c r="B36" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="8"/>
+      <c r="F36" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="5">
@@ -1208,15 +1234,18 @@
       <c r="B37" t="s">
         <v>50</v>
       </c>
+      <c r="F37" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="5">
         <v>33</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D38" t="s">

</xml_diff>